<commit_message>
added author search and sort validation
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/data/API_TestData.xlsx
+++ b/src/main/java/com/qa/data/API_TestData.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="StatusCode" sheetId="1" r:id="rId1"/>
     <sheet name="Headers" sheetId="2" r:id="rId2"/>
     <sheet name="JSONData" sheetId="3" r:id="rId3"/>
+    <sheet name="UserName" sheetId="4" r:id="rId4"/>
+    <sheet name="SortData" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>URL</t>
   </si>
@@ -100,6 +102,60 @@
   </si>
   <si>
     <t>91554</t>
+  </si>
+  <si>
+    <t>/items[0]/owner/type</t>
+  </si>
+  <si>
+    <t>Abishekk84</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>?q=user:abishekk84</t>
+  </si>
+  <si>
+    <t>StatusCode</t>
+  </si>
+  <si>
+    <t>?q=user:123abc</t>
+  </si>
+  <si>
+    <t>?q=user:123</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Validation Failed</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>total_count</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>SortParam</t>
+  </si>
+  <si>
+    <t>stars</t>
+  </si>
+  <si>
+    <t>SortOrder</t>
+  </si>
+  <si>
+    <t>asc</t>
+  </si>
+  <si>
+    <t>desc</t>
   </si>
 </sst>
 </file>
@@ -544,7 +600,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,4 +743,166 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="21" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="41.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>